<commit_message>
added final audio files
</commit_message>
<xml_diff>
--- a/modules/audio_spectrum/rev_e/audio_spectrum_bom.xlsx
+++ b/modules/audio_spectrum/rev_e/audio_spectrum_bom.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="310">
   <si>
     <t xml:space="preserve">Part</t>
   </si>
@@ -523,6 +523,9 @@
     <t xml:space="preserve">R1</t>
   </si>
   <si>
+    <t xml:space="preserve">DNP - 0</t>
+  </si>
+  <si>
     <t xml:space="preserve">RESISTOR0603_RES</t>
   </si>
   <si>
@@ -574,8 +577,7 @@
     <t xml:space="preserve">Rohm</t>
   </si>
   <si>
-    <t xml:space="preserve">MCR03ERTJ152
-</t>
+    <t xml:space="preserve">MCR03ERTJ152 </t>
   </si>
   <si>
     <t xml:space="preserve">R7</t>
@@ -1021,13 +1023,9 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1050,7 +1048,7 @@
   <dimension ref="A1:J111"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="I41" activeCellId="0" sqref="I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2381,941 +2379,941 @@
       <c r="A52" s="0" t="s">
         <v>166</v>
       </c>
-      <c r="B52" s="0" t="n">
-        <v>0</v>
+      <c r="B52" s="0" t="s">
+        <v>167</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F52" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="G52" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="I52" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F53" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="G53" s="0" t="s">
         <v>21</v>
       </c>
       <c r="I53" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F54" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="G54" s="0" t="s">
         <v>21</v>
       </c>
       <c r="I54" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="B55" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="C55" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="D55" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="E55" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="F55" s="0" t="s">
         <v>179</v>
-      </c>
-      <c r="B55" s="0" t="s">
-        <v>174</v>
-      </c>
-      <c r="C55" s="0" t="s">
-        <v>167</v>
-      </c>
-      <c r="D55" s="0" t="s">
-        <v>168</v>
-      </c>
-      <c r="E55" s="0" t="s">
-        <v>169</v>
-      </c>
-      <c r="F55" s="0" t="s">
-        <v>178</v>
       </c>
       <c r="G55" s="0" t="s">
         <v>21</v>
       </c>
       <c r="I55" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E56" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F56" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="G56" s="0" t="s">
         <v>21</v>
       </c>
       <c r="I56" s="0" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B57" s="0" t="s">
         <v>99</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F57" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="G57" s="0" t="s">
-        <v>183</v>
-      </c>
-      <c r="I57" s="1" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="58" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I57" s="0" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B58" s="0" t="s">
         <v>99</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E58" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F58" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="G58" s="0" t="s">
-        <v>183</v>
-      </c>
-      <c r="I58" s="1" t="s">
         <v>184</v>
+      </c>
+      <c r="I58" s="0" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B59" s="0" t="s">
         <v>99</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E59" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F59" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="G59" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="I59" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B60" s="0" t="s">
         <v>99</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E60" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F60" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="G60" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="I60" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E61" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F61" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="G61" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="I61" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="B62" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="C62" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="D62" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="E62" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="F62" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="G62" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="I62" s="0" t="s">
         <v>193</v>
-      </c>
-      <c r="B62" s="0" t="s">
-        <v>190</v>
-      </c>
-      <c r="C62" s="0" t="s">
-        <v>167</v>
-      </c>
-      <c r="D62" s="0" t="s">
-        <v>168</v>
-      </c>
-      <c r="E62" s="0" t="s">
-        <v>169</v>
-      </c>
-      <c r="F62" s="0" t="s">
-        <v>191</v>
-      </c>
-      <c r="G62" s="0" t="s">
-        <v>183</v>
-      </c>
-      <c r="I62" s="0" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F63" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="G63" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="I63" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F64" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="G64" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="I64" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E65" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F65" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="G65" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="I65" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E66" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F66" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="G66" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="I66" s="0" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="B67" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="C67" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="D67" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="E67" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="F67" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="G67" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="I67" s="0" t="s">
         <v>202</v>
-      </c>
-      <c r="B67" s="0" t="s">
-        <v>199</v>
-      </c>
-      <c r="C67" s="0" t="s">
-        <v>167</v>
-      </c>
-      <c r="D67" s="0" t="s">
-        <v>168</v>
-      </c>
-      <c r="E67" s="0" t="s">
-        <v>169</v>
-      </c>
-      <c r="F67" s="0" t="s">
-        <v>200</v>
-      </c>
-      <c r="G67" s="0" t="s">
-        <v>183</v>
-      </c>
-      <c r="I67" s="0" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D68" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E68" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F68" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="G68" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="I68" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
+        <v>208</v>
+      </c>
+      <c r="B69" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="C69" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="D69" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="E69" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="F69" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="G69" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="I69" s="0" t="s">
         <v>207</v>
-      </c>
-      <c r="B69" s="0" t="s">
-        <v>204</v>
-      </c>
-      <c r="C69" s="0" t="s">
-        <v>167</v>
-      </c>
-      <c r="D69" s="0" t="s">
-        <v>168</v>
-      </c>
-      <c r="E69" s="0" t="s">
-        <v>169</v>
-      </c>
-      <c r="F69" s="0" t="s">
-        <v>205</v>
-      </c>
-      <c r="G69" s="0" t="s">
-        <v>183</v>
-      </c>
-      <c r="I69" s="0" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D70" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E70" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F70" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="G70" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="I70" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D71" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E71" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F71" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="G71" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="I71" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D72" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E72" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F72" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="G72" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="I72" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D73" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E73" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F73" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="G73" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="I73" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D74" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E74" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F74" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="G74" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="I74" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D75" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E75" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F75" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="G75" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="I75" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D76" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E76" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F76" s="0" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="G76" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="I76" s="0" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D77" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E77" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F77" s="0" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="G77" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="I77" s="0" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="B78" s="0" t="s">
+        <v>220</v>
+      </c>
+      <c r="C78" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="D78" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="E78" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="F78" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="G78" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="I78" s="0" t="s">
         <v>222</v>
-      </c>
-      <c r="B78" s="0" t="s">
-        <v>219</v>
-      </c>
-      <c r="C78" s="0" t="s">
-        <v>167</v>
-      </c>
-      <c r="D78" s="0" t="s">
-        <v>168</v>
-      </c>
-      <c r="E78" s="0" t="s">
-        <v>169</v>
-      </c>
-      <c r="F78" s="0" t="s">
-        <v>220</v>
-      </c>
-      <c r="G78" s="0" t="s">
-        <v>183</v>
-      </c>
-      <c r="I78" s="0" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D79" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E79" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F79" s="0" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="G79" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="I79" s="0" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D80" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E80" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F80" s="0" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="G80" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="I80" s="0" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D81" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E81" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F81" s="0" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="G81" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="I81" s="0" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D82" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E82" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F82" s="0" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="G82" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="I82" s="0" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D83" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E83" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F83" s="0" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="G83" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="I83" s="0" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
+        <v>232</v>
+      </c>
+      <c r="B84" s="0" t="s">
+        <v>229</v>
+      </c>
+      <c r="C84" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="D84" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="E84" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="F84" s="0" t="s">
+        <v>230</v>
+      </c>
+      <c r="G84" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="I84" s="0" t="s">
         <v>231</v>
-      </c>
-      <c r="B84" s="0" t="s">
-        <v>228</v>
-      </c>
-      <c r="C84" s="0" t="s">
-        <v>167</v>
-      </c>
-      <c r="D84" s="0" t="s">
-        <v>168</v>
-      </c>
-      <c r="E84" s="0" t="s">
-        <v>169</v>
-      </c>
-      <c r="F84" s="0" t="s">
-        <v>229</v>
-      </c>
-      <c r="G84" s="0" t="s">
-        <v>183</v>
-      </c>
-      <c r="I84" s="0" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D85" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E85" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F85" s="0" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="G85" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="I85" s="0" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D86" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E86" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F86" s="0" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="G86" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="I86" s="0" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="D87" s="0" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="E87" s="0" t="s">
+        <v>242</v>
+      </c>
+      <c r="F87" s="0" t="s">
+        <v>243</v>
+      </c>
+      <c r="G87" s="0" t="s">
+        <v>244</v>
+      </c>
+      <c r="I87" s="0" t="s">
         <v>241</v>
-      </c>
-      <c r="F87" s="0" t="s">
-        <v>242</v>
-      </c>
-      <c r="G87" s="0" t="s">
-        <v>243</v>
-      </c>
-      <c r="I87" s="0" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B88" s="0" t="s">
         <v>11</v>
@@ -3335,7 +3333,7 @@
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B89" s="0" t="s">
         <v>11</v>
@@ -3355,7 +3353,7 @@
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B90" s="0" t="s">
         <v>11</v>
@@ -3375,7 +3373,7 @@
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B91" s="0" t="s">
         <v>11</v>
@@ -3395,7 +3393,7 @@
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B92" s="0" t="s">
         <v>11</v>
@@ -3415,7 +3413,7 @@
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B93" s="0" t="s">
         <v>11</v>
@@ -3435,7 +3433,7 @@
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B94" s="0" t="s">
         <v>11</v>
@@ -3455,7 +3453,7 @@
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B95" s="0" t="s">
         <v>11</v>
@@ -3475,7 +3473,7 @@
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B96" s="0" t="s">
         <v>11</v>
@@ -3495,7 +3493,7 @@
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B97" s="0" t="s">
         <v>11</v>
@@ -3515,7 +3513,7 @@
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B98" s="0" t="s">
         <v>11</v>
@@ -3535,7 +3533,7 @@
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B99" s="0" t="s">
         <v>11</v>
@@ -3555,7 +3553,7 @@
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B100" s="0" t="s">
         <v>11</v>
@@ -3575,288 +3573,288 @@
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B101" s="0" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C101" s="0" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="D101" s="0" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="E101" s="0" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="F101" s="0" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="G101" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="I101" s="0" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B102" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C102" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D102" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="E102" s="0" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="F102" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="G102" s="0" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="I102" s="0" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B103" s="0" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C103" s="0" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="D103" s="0" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="E103" s="0" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="F103" s="0" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="G103" s="0" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="I103" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
+        <v>278</v>
+      </c>
+      <c r="B104" s="0" t="s">
+        <v>272</v>
+      </c>
+      <c r="C104" s="0" t="s">
+        <v>272</v>
+      </c>
+      <c r="D104" s="0" t="s">
+        <v>273</v>
+      </c>
+      <c r="E104" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="F104" s="0" t="s">
+        <v>275</v>
+      </c>
+      <c r="G104" s="0" t="s">
+        <v>276</v>
+      </c>
+      <c r="I104" s="0" t="s">
         <v>277</v>
-      </c>
-      <c r="B104" s="0" t="s">
-        <v>271</v>
-      </c>
-      <c r="C104" s="0" t="s">
-        <v>271</v>
-      </c>
-      <c r="D104" s="0" t="s">
-        <v>272</v>
-      </c>
-      <c r="E104" s="0" t="s">
-        <v>273</v>
-      </c>
-      <c r="F104" s="0" t="s">
-        <v>274</v>
-      </c>
-      <c r="G104" s="0" t="s">
-        <v>275</v>
-      </c>
-      <c r="I104" s="0" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B105" s="0" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C105" s="0" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D105" s="0" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="E105" s="0" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="F105" s="0" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="G105" s="0" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="I105" s="0" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
+        <v>286</v>
+      </c>
+      <c r="B106" s="0" t="s">
+        <v>280</v>
+      </c>
+      <c r="C106" s="0" t="s">
+        <v>280</v>
+      </c>
+      <c r="D106" s="0" t="s">
+        <v>281</v>
+      </c>
+      <c r="E106" s="0" t="s">
+        <v>282</v>
+      </c>
+      <c r="F106" s="0" t="s">
+        <v>283</v>
+      </c>
+      <c r="G106" s="0" t="s">
+        <v>284</v>
+      </c>
+      <c r="I106" s="0" t="s">
         <v>285</v>
-      </c>
-      <c r="B106" s="0" t="s">
-        <v>279</v>
-      </c>
-      <c r="C106" s="0" t="s">
-        <v>279</v>
-      </c>
-      <c r="D106" s="0" t="s">
-        <v>280</v>
-      </c>
-      <c r="E106" s="0" t="s">
-        <v>281</v>
-      </c>
-      <c r="F106" s="0" t="s">
-        <v>282</v>
-      </c>
-      <c r="G106" s="0" t="s">
-        <v>283</v>
-      </c>
-      <c r="I106" s="0" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B107" s="0" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C107" s="0" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D107" s="0" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="E107" s="0" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="F107" s="0" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="G107" s="0" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="I107" s="0" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B108" s="0" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C108" s="0" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D108" s="0" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="E108" s="0" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="F108" s="0" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="G108" s="0" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="I108" s="0" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B109" s="0" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="C109" s="0" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D109" s="0" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="E109" s="0" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="F109" s="0" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="G109" s="0" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="I109" s="0" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B110" s="0" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C110" s="0" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="D110" s="0" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="E110" s="0" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="F110" s="0" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="G110" s="0" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="I110" s="0" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B111" s="0" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C111" s="0" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="D111" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="E111" s="0" t="s">
+        <v>307</v>
+      </c>
+      <c r="F111" s="0" t="s">
+        <v>308</v>
+      </c>
+      <c r="G111" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="I111" s="0" t="s">
         <v>305</v>
-      </c>
-      <c r="E111" s="0" t="s">
-        <v>306</v>
-      </c>
-      <c r="F111" s="0" t="s">
-        <v>307</v>
-      </c>
-      <c r="G111" s="0" t="s">
-        <v>308</v>
-      </c>
-      <c r="I111" s="0" t="s">
-        <v>304</v>
       </c>
     </row>
   </sheetData>

</xml_diff>